<commit_message>
Connected UI to the generate maze script
</commit_message>
<xml_diff>
--- a/Documents/DTT-Assessment-Hour-Log.xlsx
+++ b/Documents/DTT-Assessment-Hour-Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26105"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80D0B132-86D1-4FCE-90ED-1F0CA345914A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FB819B3-149E-4B79-B958-7D93042124B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Uur</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Ik heb een UI toegevoegd aan de generator. Op het moment zit deze nog niet aangesloten aan het generate script. Daarnaast heb ik particles toegevoegd die om de vorm van de maze zitten. Als laatste heb ik nog wat code gescheven die op random plekken boven en onder aan het doolhof en ingang en uitgang plaatst.</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Dit uur was iets minder prodcutief. Ik heb de UI gebonden aan het generate script, en er gelijk voor gezorgd dat de user pas een doolhoof kan genereren als alle input velden een getal hebben. de functie om een doolhof te maken door op "G" te klikken is verwijderd.</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,6 +487,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="20" ht="7.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added FX to cells on the borders and cells spawning in, added maximum values to UI
</commit_message>
<xml_diff>
--- a/Documents/DTT-Assessment-Hour-Log.xlsx
+++ b/Documents/DTT-Assessment-Hour-Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26105"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FB819B3-149E-4B79-B958-7D93042124B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{40ADA218-B83E-4145-9B35-6C1FACE6BC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Uur</t>
   </si>
@@ -61,13 +61,35 @@
   </si>
   <si>
     <t>Dit uur was iets minder prodcutief. Ik heb de UI gebonden aan het generate script, en er gelijk voor gezorgd dat de user pas een doolhoof kan genereren als alle input velden een getal hebben. de functie om een doolhof te maken door op "G" te klikken is verwijderd.</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Officieel klaar met de user stories!! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Dit uur heb ik ervoor gezorgd dat er particle effects worden gegeven aan de cells op de rand van de maze, en er word nu een animatie gespeeld wanneer een cell op beeld komt. Ik heb ook een maximum ingesteld zodat de X en Y niet groter kunnen zijn dan 250. het maken van de maze op deze grote is echter niet aan te raden. Ik kom hier later op terug in het README document. De user kan nu ook een nieuwe maze aanmaken waarneer die wilt.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +106,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -109,13 +137,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -432,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -498,6 +527,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="20" ht="7.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added pretty mode, added meme, added dynamic camera positioning
</commit_message>
<xml_diff>
--- a/Documents/DTT-Assessment-Hour-Log.xlsx
+++ b/Documents/DTT-Assessment-Hour-Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26105"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40ADA218-B83E-4145-9B35-6C1FACE6BC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4876590C-CA9C-4EB7-A201-4E5D85A471D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Uur</t>
   </si>
@@ -83,6 +83,12 @@
       </rPr>
       <t>Dit uur heb ik ervoor gezorgd dat er particle effects worden gegeven aan de cells op de rand van de maze, en er word nu een animatie gespeeld wanneer een cell op beeld komt. Ik heb ook een maximum ingesteld zodat de X en Y niet groter kunnen zijn dan 250. het maken van de maze op deze grote is echter niet aan te raden. Ik kom hier later op terug in het README document. De user kan nu ook een nieuwe maze aanmaken waarneer die wilt.</t>
     </r>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Dit uur heb ik als eerste een meme toegevoegd als je het project opent. Daarna heb ik een "Pretty mode" button gemaakt. Deze activeerd / deactiveerd de return yield null in de GenerateScript IEnumerator. Hierdoor is er of instant een maze gegenereerd, of visueel stapje voor stapje. als laatste heb ik een klein stukje code toegevoeg zodat de start positie van de camera gebaseerd is op de grote van de maze. Hierdoor zie je altijd de hele maze aan het begin.</t>
   </si>
 </sst>
 </file>
@@ -461,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -538,6 +544,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="2"/>
+    </row>
     <row r="20" ht="7.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more options, fixed double maze generation bug
</commit_message>
<xml_diff>
--- a/Documents/DTT-Assessment-Hour-Log.xlsx
+++ b/Documents/DTT-Assessment-Hour-Log.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26111"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4876590C-CA9C-4EB7-A201-4E5D85A471D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94DBCCD9-A0FE-4591-9DB4-01F017A8CF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Uur</t>
   </si>
@@ -73,7 +73,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">Officieel klaar met de user stories!! </t>
+      <t xml:space="preserve">Officieel klaar met de user stories!! in versie 2.1 zijn echter alle bugs er pas uit.  </t>
     </r>
     <r>
       <rPr>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Dit uur heb ik als eerste een meme toegevoegd als je het project opent. Daarna heb ik een "Pretty mode" button gemaakt. Deze activeerd / deactiveerd de return yield null in de GenerateScript IEnumerator. Hierdoor is er of instant een maze gegenereerd, of visueel stapje voor stapje. als laatste heb ik een klein stukje code toegevoeg zodat de start positie van de camera gebaseerd is op de grote van de maze. Hierdoor zie je altijd de hele maze aan het begin.</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Ik heb 2 extra opties toegevoegd om performance te verbeteren bij grote mazes. Eentje op het licht uit te zetten, en de andere om de particles uit te zetten. De  "Pretty mode" functie heet nu "Fast mode" voor verduiderlijking. Hiernaast heb ik code geschreven zodat de oude cells die nog gegenereerd werden allemaal verwijderd worden, doormiddel van StopCoroutine. Hiervoor  gebeurde dit niet altijd.</t>
   </si>
 </sst>
 </file>
@@ -468,7 +474,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -556,7 +562,15 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="B8" s="2"/>
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" ht="7.5" customHeight="1"/>
   </sheetData>

</xml_diff>

<commit_message>
Fixed no perfect maze issue
</commit_message>
<xml_diff>
--- a/Documents/DTT-Assessment-Hour-Log.xlsx
+++ b/Documents/DTT-Assessment-Hour-Log.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timva\OneDrive\Bureaublad\Maze\Maze-Genetator\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F0279D-DEAF-43A9-A88C-A6D8EFCB7499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E05D01D-5953-4E6E-98D5-047256C3B1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +24,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -34,25 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Amount of hours</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Total amount of hours</t>
-  </si>
-  <si>
-    <t>Bonus</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <r>
       <rPr>
@@ -76,49 +60,73 @@
     </r>
   </si>
   <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Amount of hours</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Creating the first itteration of the Maze Generation Algorithm</t>
+  </si>
+  <si>
     <t>I started and finsihed the first itteration of the maze algorithm this hour. I decided to follow a youtube tutorial about Depth-First-Search, the video is linked in my included README file. I found found it quite easy to follow and to understand how the algortihm worked.</t>
   </si>
   <si>
+    <t>Implementing special FX and animations</t>
+  </si>
+  <si>
     <t>14/01/2023</t>
   </si>
   <si>
-    <t>Creating the first itteration of the Maze Generation Algorithm</t>
-  </si>
-  <si>
-    <t>Implementing special FX and animations</t>
+    <t>The project so far was looking a bit bland for my taste, so I decided to dedicade some time to animation and FX. In these 2 hours I added the following this: Particle effects around the maze, No Mazes? Meme and a cell instantiate animation. I did not run into any issues as i have done these things before. Picking out a nice special effect and searching for cool assets took some time. I used to instantiate a particle effect on every cell, but later i realized that this was a waste of recources. I simple wrote an if statement to instantie a effect if the current cell was on the border of the X and / or y maximum or minimum value.</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Building and connecting the UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This took longer than i expected, especially  because I had build UI for my other projects before. It took this long because i never made my UI's responsive, so I needed to figure this out first. I also had to alter the UI everytime I added features to improve performance. </t>
+  </si>
+  <si>
+    <t>Implemented user stories</t>
+  </si>
+  <si>
+    <t>I already had most of the user stories completed when I finished the algorithm. I even misread the pdf and added a feature to increase the wallheight of the maze. All i needed to add at this point were: max Y and X size, min X and Y size and to make the user be able to regenerate the maze anytime. Implementing a max and min value was quite quickely done using a simple if statement. The regeneration feature took some time tho. I did not know about the StopCoroutine() function yet, so it took some time to figure out how to stop the previous maze coroutine form running.</t>
+  </si>
+  <si>
+    <t>Building the  second iteration of algorithm to increase speed</t>
   </si>
   <si>
     <t>16/01/2023</t>
   </si>
   <si>
-    <t>X</t>
+    <t>This was by far my biggest "waste" of time in this project. I tried to look for ways to get the overall generation time down for larger mazes, because it took 12 seconds to load a 150 x 150 :(. I tried object pooling, but this caused my program to crash alot becasue it had to load in 62,500 3d object beforehand (a 250 x 250 maze). That obviously was not going to work. I tried to instantiate a random amount of cells with missing walls, but this was not improving performance alot and it looked bad. I sadly never figured a way out to increase the overall speed of the maze generation</t>
+  </si>
+  <si>
+    <t>Testing out ways to increase performance</t>
   </si>
   <si>
     <t>I noticed that the algorithm wasn't fast when the user wanted t o create large mazes (above 50 x 50). After some thinking I decided to add extra "Maze Runners" so the actual creating of the pase pattern would be quicker. This was not possible with the first itteration of the algorithm because the lists with cells were created by the single maze runner. I decided to create a seperate prefab and script for the maze runner, so i could instantiate more of them. I needed to alter their script so they would send en recieve their lists with altered cells to the maze generator. This would prevent the maze walkers from checking cells that already were altered by other maze walkers. I sadly ran into an error message that i could not / did not have the knowledge to fix. Apparently the maze runners are set to inactive after they get instantiated. This prevented the StartMazeRunner() Coroutine from running. I tried mulitple possibilies, but even with gameObject.SetActive(true) the coroutine would not run. This ultimately increased the speed by a little bit.</t>
   </si>
   <si>
-    <t>Building the  second iteration of algorithm to increase speed</t>
-  </si>
-  <si>
-    <t>Testing out ways to increase performance</t>
-  </si>
-  <si>
-    <t>The project so far was looking a bit bland for my taste, so I decided to dedicade some time to animation and FX. In these 2 hours I added the following this: Particle effects around the maze, No Mazes? Meme and a cell instantiate animation. I did not run into any issues as i have done these things before. Picking out a nice special effect and searching for cool assets took some time. I used to instantiate a particle effect on every cell, but later i realized that this was a waste of recources. I simple wrote an if statement to instantie a effect if the current cell was on the border of the X and / or y maximum or minimum value.</t>
-  </si>
-  <si>
-    <t>This was by far my biggest "waste" of time in this project. I tried to look for ways to get the overall generation time down for larger mazes, because it took 12 seconds to load a 150 x 150 :(. I tried object pooling, but this caused my program to crash alot becasue it had to load in 62,500 3d object beforehand (a 250 x 250 maze). That obviously was not going to work. I tried to instantiate a random amount of cells with missing walls, but this was not improving performance alot and it looked bad. I sadly never figured a way out to increase the overall speed of the maze generation</t>
-  </si>
-  <si>
-    <t>Building and connecting the UI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This took longer than i expected, especially  because I had build UI for my other projects before. It took this long because i never made my UI's responsive, so I needed to figure this out first. I also had to alter the UI everytime I added features to improve performance. </t>
-  </si>
-  <si>
-    <t>Implemented user stories</t>
-  </si>
-  <si>
-    <t>I already had most of the user stories completed when I finished the algorithm. I even misread the pdf and added a feature to increase the wallheight of the maze. All i needed to add at this point were: max Y and X size, min X and Y size and to make the user be able to regenerate the maze anytime. Implementing a max and min value was quite quickely done using a simple if statement. The regeneration feature took some time tho. I did not know about the StopCoroutine() function yet, so it took some time to figure out how to stop the previous maze coroutine form running.</t>
+    <t>Fixing no perfect maze option</t>
+  </si>
+  <si>
+    <t>Ater running a few test, i noticed that the algortihm did not always produce a "perfect maze". I later found out that this had to do with runnig multiple maze runners at the same time. Somehow the index of the cells in the currentCellPath did not always align. That is why i decided to only use 1 maze runner for now, but also still keep the same code structure. This way i could easily add more maze runners in the future, for when i have fixed the alignment issue.</t>
+  </si>
+  <si>
+    <t>Total amount of hours</t>
   </si>
 </sst>
 </file>
@@ -128,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1732,11 +1740,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="24.69921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.69921875" style="1" customWidth="1"/>
@@ -1746,7 +1754,7 @@
     <col min="7" max="251" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="73.5" customHeight="1">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1754,9 +1762,9 @@
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="46.5" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1764,27 +1772,27 @@
       <c r="E2" s="23"/>
       <c r="F2" s="24"/>
     </row>
-    <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="17">
         <v>1</v>
@@ -1798,96 +1806,104 @@
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="B6" s="17">
         <v>1</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7" s="17">
         <v>1</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="17">
         <v>4</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="15"/>
+    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="17">
+        <v>2</v>
+      </c>
+      <c r="C10" s="18">
+        <v>44943</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
@@ -1895,7 +1911,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1903,7 +1919,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
@@ -1911,7 +1927,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -1919,7 +1935,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -1927,7 +1943,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -1935,7 +1951,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -1943,7 +1959,7 @@
       <c r="E17" s="20"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -1951,7 +1967,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="5"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18"/>
@@ -1959,7 +1975,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1967,7 +1983,7 @@
       <c r="E20" s="20"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1975,7 +1991,7 @@
       <c r="E21" s="20"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18"/>
@@ -1983,7 +1999,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
@@ -1991,7 +2007,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
@@ -1999,7 +2015,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
@@ -2007,7 +2023,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
@@ -2015,7 +2031,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
@@ -2023,7 +2039,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
@@ -2031,7 +2047,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="16.350000000000001" customHeight="1">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2039,20 +2055,20 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="16.350000000000001" customHeight="1">
       <c r="A30" s="13" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="16.350000000000001" customHeight="1">
       <c r="A31" s="6"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2060,7 +2076,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="16.350000000000001" customHeight="1">
       <c r="A32" s="6"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2068,7 +2084,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="16.350000000000001" customHeight="1">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>

</xml_diff>